<commit_message>
Fix user branch selection and add notification for branch orders
</commit_message>
<xml_diff>
--- a/src/public/Rizq #1.xlsx
+++ b/src/public/Rizq #1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Nomi</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Виноград 6</t>
+  </si>
+  <si>
+    <t>яблоко 8</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -523,7 +526,7 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="C9" s="1">
         <v>45342.36532946759</v>
@@ -549,6 +552,17 @@
       </c>
       <c r="C11" s="1">
         <v>45343.369962743054</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>55</v>
+      </c>
+      <c r="C12" s="1">
+        <v>45343.68824604167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>